<commit_message>
too much info in file
</commit_message>
<xml_diff>
--- a/chapter1.xlsx
+++ b/chapter1.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeandaniel/Documents/numerical_approx_methods/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeandaniel/Documents/GitHub/numerical_approx_methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7D27F0-A6BA-8845-ADF9-A0D1A6B479D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE85839-939F-5E4B-B976-DBAC9F85930C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="1520" windowWidth="28800" windowHeight="17500" xr2:uid="{229481EE-D526-4287-B445-7343DE9ED797}"/>
+    <workbookView xWindow="6040" yWindow="1300" windowWidth="28800" windowHeight="17500" xr2:uid="{229481EE-D526-4287-B445-7343DE9ED797}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Boulder" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="71">
   <si>
     <t>lagrange interpolation</t>
   </si>
@@ -217,27 +216,6 @@
   </si>
   <si>
     <t>y(x)</t>
-  </si>
-  <si>
-    <t>Saturday</t>
-  </si>
-  <si>
-    <t>Sunday</t>
-  </si>
-  <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t>Tuesday</t>
-  </si>
-  <si>
-    <t>Wednesday</t>
-  </si>
-  <si>
-    <t>Thursday</t>
-  </si>
-  <si>
-    <t>Friday</t>
   </si>
   <si>
     <t>Approximate for |x| &lt; 1</t>
@@ -5023,335 +5001,6 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Bould-it road to 60mi</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Boulder!$A$1:$A$7</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>Saturday</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Sunday</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Monday</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Tuesday</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Wednesday</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Thursday</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Friday</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Boulder!$B$1:$B$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
-                <c:pt idx="0">
-                  <c:v>21.29</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.33</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16.73</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.71</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>21.27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>11.44</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4A63-584D-A671-D43C1BB46EDD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="149909567"/>
-        <c:axId val="149911887"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="149909567"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="149911887"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="149911887"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="21"/>
-          <c:min val="0"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="149909567"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="3"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -5672,46 +5321,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -9821,509 +9430,6 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style9.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -14078,47 +13184,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E54C3551-8ACB-1B06-100A-B3AF2786A89B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -15561,7 +14626,7 @@
         <v>55</v>
       </c>
       <c r="B138" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -15792,13 +14857,13 @@
     </row>
     <row r="165" spans="2:8">
       <c r="B165" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E165" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="G165" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="166" spans="2:8">
@@ -15809,7 +14874,7 @@
         <v>59</v>
       </c>
       <c r="E166" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="G166" t="s">
         <v>1</v>
@@ -15827,7 +14892,7 @@
         <v>-0.99999999997301514</v>
       </c>
       <c r="E167" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G167">
         <v>-2</v>
@@ -15846,7 +14911,7 @@
         <v>-0.99802718046162175</v>
       </c>
       <c r="E168" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="G168">
         <v>-1.9</v>
@@ -15881,7 +14946,7 @@
         <v>-0.98228854469046911</v>
       </c>
       <c r="E170" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="F170">
         <v>1</v>
@@ -15903,7 +14968,7 @@
         <v>-0.96858484192619998</v>
       </c>
       <c r="E171" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F171">
         <f>SIN(0)</f>
@@ -15926,7 +14991,7 @@
         <v>-0.951058559423407</v>
       </c>
       <c r="E172" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="F172">
         <f>-COS(0)</f>
@@ -15949,7 +15014,7 @@
         <v>-0.92977886573551638</v>
       </c>
       <c r="E173" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F173">
         <f>SIN(0)</f>
@@ -17056,85 +16121,4 @@
   </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFA73656-A101-5C48-979C-2515DF29B127}">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1">
-        <v>21.29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2">
-        <v>8.33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
-        <v>16.73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>63</v>
-      </c>
-      <c r="B4">
-        <v>7.71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B5">
-        <v>21.27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6">
-        <v>11.44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="B8">
-        <f>SUM(B1:B7)</f>
-        <v>86.77</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Runge Kutta single step works with error plot
</commit_message>
<xml_diff>
--- a/chapter1.xlsx
+++ b/chapter1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeandaniel/Documents/GitHub/numerical_approx_methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2393D3D7-293C-754E-9681-05F0D9C97922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D7D21C-170D-934C-8D2A-A53453194B82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="2300" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{229481EE-D526-4287-B445-7343DE9ED797}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
   <si>
     <t>lagrange interpolation</t>
   </si>
@@ -322,6 +322,9 @@
   </si>
   <si>
     <t>RK</t>
+  </si>
+  <si>
+    <t>xn</t>
   </si>
 </sst>
 </file>
@@ -18699,10 +18702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69D36FDF-279F-9041-B29C-3E803722C1EA}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -18786,7 +18789,7 @@
         <v>0.3</v>
       </c>
       <c r="D14" t="s">
-        <v>1</v>
+        <v>95</v>
       </c>
       <c r="E14" t="s">
         <v>94</v>
@@ -18814,15 +18817,8 @@
       <c r="B16">
         <v>3</v>
       </c>
-      <c r="D16">
-        <v>0.1</v>
-      </c>
-      <c r="E16">
-        <f t="shared" ref="E16:E45" si="0">$B$16+1/6*($B$17+2*$B$18+2*$B$19+$B$20)</f>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -18830,15 +18826,8 @@
         <f>((B15)^2)*((B16^2))*0.3</f>
         <v>0</v>
       </c>
-      <c r="D17">
-        <v>0.2</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -18846,15 +18835,8 @@
         <f>(($B$15+1/2*$B$14)^2*($B$16+1/2*B17)^2)*$B$14</f>
         <v>6.0749999999999992E-2</v>
       </c>
-      <c r="D18">
-        <v>0.3</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>79</v>
       </c>
@@ -18862,253 +18844,14 @@
         <f>(($B$15+1/2*$B$14)^2*($B$16+1/2*B18)^2)*$B$14</f>
         <v>6.1986415324218738E-2</v>
       </c>
-      <c r="D19">
-        <v>0.4</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>80</v>
       </c>
       <c r="B20">
         <f>(B15+B14)^2*(B16+B19)^2*B14</f>
         <v>0.25314554180601156</v>
-      </c>
-      <c r="D20">
-        <v>0.5</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="D21">
-        <v>0.6</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="D22">
-        <v>0.7</v>
-      </c>
-      <c r="E22">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="D23">
-        <v>0.8</v>
-      </c>
-      <c r="E23">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="D24">
-        <v>0.9</v>
-      </c>
-      <c r="E24">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="D26">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="D27">
-        <v>1.2</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="D28">
-        <v>1.3</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="D29">
-        <v>1.4</v>
-      </c>
-      <c r="E29">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="D30">
-        <v>1.5</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="D31">
-        <v>1.6</v>
-      </c>
-      <c r="E31">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="D32">
-        <v>1.7</v>
-      </c>
-      <c r="E32">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="33" spans="4:5">
-      <c r="D33">
-        <v>1.8</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="34" spans="4:5">
-      <c r="D34">
-        <v>1.9</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="35" spans="4:5">
-      <c r="D35">
-        <v>2</v>
-      </c>
-      <c r="E35">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="36" spans="4:5">
-      <c r="D36">
-        <v>2.1</v>
-      </c>
-      <c r="E36">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="37" spans="4:5">
-      <c r="D37">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="E37">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="38" spans="4:5">
-      <c r="D38">
-        <v>2.2999999999999998</v>
-      </c>
-      <c r="E38">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="39" spans="4:5">
-      <c r="D39">
-        <v>2.4</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="40" spans="4:5">
-      <c r="D40">
-        <v>2.5</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="41" spans="4:5">
-      <c r="D41">
-        <v>2.6</v>
-      </c>
-      <c r="E41">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="42" spans="4:5">
-      <c r="D42">
-        <v>2.7</v>
-      </c>
-      <c r="E42">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="43" spans="4:5">
-      <c r="D43">
-        <v>2.8</v>
-      </c>
-      <c r="E43">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="44" spans="4:5">
-      <c r="D44">
-        <v>2.9</v>
-      </c>
-      <c r="E44">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
-      </c>
-    </row>
-    <row r="45" spans="4:5">
-      <c r="D45">
-        <v>3</v>
-      </c>
-      <c r="E45">
-        <f t="shared" si="0"/>
-        <v>3.0831030620757414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>